<commit_message>
inca un save sa nu uite uipath
</commit_message>
<xml_diff>
--- a/DateInstagram.xlsx
+++ b/DateInstagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tamina\Documents\UiPath\Proiect RPA Zamfir Tamina\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD473BBD-1FE9-4AFC-BE4E-E4E3D076EC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F7FBA4-DF87-4D54-9187-B6031FE2A9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" firstSheet="0" activeTab="1" xr2:uid="{42BB713D-70BA-47E1-99D9-6DBF6DCE9DCC}"/>
   </x:bookViews>
@@ -538,7 +538,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D2"/>
+  <x:dimension ref="A1:D5"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
       <x:selection activeCell="B5" sqref="B5"/>
@@ -580,7 +580,7 @@
         <x:v>46035.0179499306</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:4">
+    <x:row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <x:c r="A3" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
@@ -594,7 +594,7 @@
         <x:v>46035.0194877431</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:4">
+    <x:row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <x:c r="A4" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
@@ -608,7 +608,7 @@
         <x:v>46035.0195843519</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:4">
+    <x:row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <x:c r="A5" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
@@ -620,6 +620,48 @@
       </x:c>
       <x:c r="D5" s="3">
         <x:v>46035.019619213</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:4">
+      <x:c r="A6" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D6" s="3">
+        <x:v>46035.0402861227</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:4">
+      <x:c r="A7" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D7" s="3">
+        <x:v>46035.0403193634</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:4">
+      <x:c r="A8" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D8" s="3">
+        <x:v>46035.0403602083</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
inca un commit ca nu am mai dat de mult timp
</commit_message>
<xml_diff>
--- a/DateInstagram.xlsx
+++ b/DateInstagram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tamina\Documents\UiPath\Proiect RPA Zamfir Tamina\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F7FBA4-DF87-4D54-9187-B6031FE2A9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB0A724-9F41-431B-9ADB-2245865D4FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" firstSheet="0" activeTab="1" xr2:uid="{42BB713D-70BA-47E1-99D9-6DBF6DCE9DCC}"/>
+    <x:workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="0" activeTab="1" xr2:uid="{42BB713D-70BA-47E1-99D9-6DBF6DCE9DCC}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="instagram" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <x:si>
     <x:t>Id</x:t>
   </x:si>
@@ -65,7 +65,7 @@
     <x:t>Va multumim de paticipare, ca urmare apasati pe linkul pentru o recompensa</x:t>
   </x:si>
   <x:si>
-    <x:t>trimis</x:t>
+    <x:t>mesaj</x:t>
   </x:si>
   <x:si>
     <x:t>id_postare</x:t>
@@ -80,10 +80,19 @@
     <x:t>data_reply</x:t>
   </x:si>
   <x:si>
+    <x:t>tip_interact</x:t>
+  </x:si>
+  <x:si>
+    <x:t>abc</x:t>
+  </x:si>
+  <x:si>
     <x:t>skiuileuf</x:t>
   </x:si>
   <x:si>
     <x:t>Alt comentariu de test care contine RPA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>message</x:t>
   </x:si>
   <x:si>
     <x:t>taminandreea</x:t>
@@ -475,9 +484,7 @@
   </x:sheetPr>
   <x:dimension ref="A1:E2"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0">
-      <x:selection activeCell="C1" sqref="C1"/>
-    </x:sheetView>
+    <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <x:cols>
@@ -523,7 +530,7 @@
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="B2" r:id="rId8"/>
+    <x:hyperlink ref="B2" r:id="rId7"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -538,21 +545,21 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D5"/>
+  <x:dimension ref="A1:E17"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="B5" sqref="B5"/>
+      <x:selection activeCell="F7" sqref="F7"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <x:cols>
     <x:col min="1" max="1" width="9.109375" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="14.664062" style="0" bestFit="1" customWidth="1"/>
-    <x:col min="3" max="3" width="11.109375" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="33.886719" style="0" bestFit="1" customWidth="1"/>
     <x:col min="4" max="4" width="15.21875" style="0" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <x:row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <x:c r="A1" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
@@ -565,104 +572,155 @@
       <x:c r="D1" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <x:c r="E1" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <x:c r="A2" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="D2" s="3">
-        <x:v>46035.0179499306</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <x:c r="D2" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6">
       <x:c r="A3" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D3" s="3">
-        <x:v>46035.0194877431</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <x:v>46035.0853269444</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6">
       <x:c r="A4" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="D4" s="3">
-        <x:v>46035.0195843519</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <x:v>46035.0853304282</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6">
       <x:c r="A5" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="D5" s="3">
-        <x:v>46035.019619213</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:4">
+        <x:v>46035.0853308912</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6">
       <x:c r="A6" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D6" s="3">
-        <x:v>46035.0402861227</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:4">
+        <x:v>46035.0855535764</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6">
       <x:c r="A7" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="D7" s="3">
-        <x:v>46035.0403193634</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:4">
+        <x:v>46035.0855568981</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <x:c r="A8" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="D8" s="3">
-        <x:v>46035.0403602083</x:v>
-      </x:c>
+        <x:v>46035.0855573611</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <x:c r="D9" s="3" t="s"/>
+    </x:row>
+    <x:row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <x:c r="D10" s="3" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <x:c r="D11" s="3" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <x:c r="D12" s="3" t="s"/>
+    </x:row>
+    <x:row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <x:c r="D13" s="3" t="s"/>
+    </x:row>
+    <x:row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <x:c r="D14" s="3" t="s"/>
+    </x:row>
+    <x:row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <x:c r="D15" s="3" t="s"/>
+    </x:row>
+    <x:row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <x:c r="D16" s="3" t="s"/>
+    </x:row>
+    <x:row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <x:c r="D17" s="3" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>